<commit_message>
sidebar & header translation
</commit_message>
<xml_diff>
--- a/skowly-ui/src/assets/i18n/i18n.xlsx
+++ b/skowly-ui/src/assets/i18n/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghass\Desktop\skowly-workspace\Skowly\skowly-ui\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A5A8FF-46BD-4B83-93FF-81F380A396DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF1073D-CCB4-4CE6-90D7-A3F1391B0F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{289BA3EF-4839-4939-93A8-DD74B1A93143}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289BA3EF-4839-4939-93A8-DD74B1A93143}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>feature</t>
   </si>
@@ -151,6 +151,144 @@
   </si>
   <si>
     <t>roles</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
+    <t>الإنجليزية</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>الفرنسية</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>Arabe</t>
+  </si>
+  <si>
+    <t>العربية</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>القائمة</t>
+  </si>
+  <si>
+    <t>sidebar</t>
+  </si>
+  <si>
+    <t>selectAnotherStudent</t>
+  </si>
+  <si>
+    <t>Select Another Student</t>
+  </si>
+  <si>
+    <t>Sélectionnez un autre étudiant</t>
+  </si>
+  <si>
+    <t>إختيار طالب آخر</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Schools</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Academic &amp; Attendance</t>
+  </si>
+  <si>
+    <t>Fees &amp; Payments</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>schools</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>calendar</t>
+  </si>
+  <si>
+    <t>academicAndAttendance</t>
+  </si>
+  <si>
+    <t>feesAndPayments</t>
+  </si>
+  <si>
+    <t>Accueil</t>
+  </si>
+  <si>
+    <t>الرئيسيّة</t>
+  </si>
+  <si>
+    <t>المدارس</t>
+  </si>
+  <si>
+    <t>Écoles</t>
+  </si>
+  <si>
+    <t>الملف الشخصي</t>
+  </si>
+  <si>
+    <t>profileDetails</t>
+  </si>
+  <si>
+    <t>Profile Details</t>
+  </si>
+  <si>
+    <t>Détails du profil</t>
+  </si>
+  <si>
+    <t>Cours</t>
+  </si>
+  <si>
+    <t>الدروس</t>
+  </si>
+  <si>
+    <t>Calendrier</t>
+  </si>
+  <si>
+    <t>التقويم</t>
+  </si>
+  <si>
+    <t>التفاصيل الأكاديمية والحضور</t>
+  </si>
+  <si>
+    <t>Détails académiques &amp; Présence</t>
+  </si>
+  <si>
+    <t>Frais &amp; Paiements</t>
+  </si>
+  <si>
+    <t>الرسوم والمدفوعات</t>
   </si>
 </sst>
 </file>
@@ -200,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -288,11 +426,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -301,15 +452,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,6 +464,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,20 +792,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B996B9F-A61E-4BAD-8E2D-6424C36803EE}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="8" customWidth="1"/>
-    <col min="4" max="4" width="35.88671875" style="9" customWidth="1"/>
-    <col min="5" max="6" width="36.44140625" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="10"/>
+    <col min="1" max="1" width="15.5546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" style="6" customWidth="1"/>
+    <col min="5" max="6" width="36.44140625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -675,141 +829,342 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="A2:A21"/>
     <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B10:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix CI/CD + some css
</commit_message>
<xml_diff>
--- a/skowly-ui/src/assets/i18n/i18n.xlsx
+++ b/skowly-ui/src/assets/i18n/i18n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghass\Desktop\skowly-workspace\Skowly\skowly-ui\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF1073D-CCB4-4CE6-90D7-A3F1391B0F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B1FEC-8696-460B-8F24-BCE5C1E99BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289BA3EF-4839-4939-93A8-DD74B1A93143}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>وليّ</t>
   </si>
   <si>
-    <t>موظف بالمدرسة</t>
-  </si>
-  <si>
     <t>مدير المدرسة</t>
   </si>
   <si>
@@ -289,6 +286,9 @@
   </si>
   <si>
     <t>الرسوم والمدفوعات</t>
+  </si>
+  <si>
+    <t>موظّف بالمدرسة</t>
   </si>
 </sst>
 </file>
@@ -466,17 +466,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,7 +795,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -829,11 +829,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>38</v>
+      <c r="B2" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -849,8 +849,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
@@ -865,8 +865,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
@@ -877,12 +877,12 @@
         <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
@@ -893,12 +893,12 @@
         <v>28</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
@@ -909,12 +909,12 @@
         <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
@@ -929,8 +929,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
@@ -945,7 +945,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="10"/>
       <c r="C9" s="5" t="s">
         <v>25</v>
@@ -961,201 +961,201 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8" t="s">
-        <v>39</v>
+      <c r="A10" s="11"/>
+      <c r="B10" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="10"/>
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="7" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8" t="s">
+      <c r="D13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="7" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="E15" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="E16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="5" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="5" t="s">
+      <c r="F18" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="5" t="s">
+      <c r="F19" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="E20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>83</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
language dropdown + some other improvements
</commit_message>
<xml_diff>
--- a/skowly-ui/src/assets/i18n/i18n.xlsx
+++ b/skowly-ui/src/assets/i18n/i18n.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghass\Desktop\skowly-workspace\Skowly\skowly-ui\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B1FEC-8696-460B-8F24-BCE5C1E99BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90483841-6515-40C9-B487-0302FD6EF69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{289BA3EF-4839-4939-93A8-DD74B1A93143}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{289BA3EF-4839-4939-93A8-DD74B1A93143}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
   <si>
     <t>feature</t>
   </si>
@@ -156,25 +156,7 @@
     <t>English</t>
   </si>
   <si>
-    <t>Anglais</t>
-  </si>
-  <si>
-    <t>الإنجليزية</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>الفرنسية</t>
-  </si>
-  <si>
     <t>Français</t>
-  </si>
-  <si>
-    <t>Arabic</t>
-  </si>
-  <si>
-    <t>Arabe</t>
   </si>
   <si>
     <t>العربية</t>
@@ -795,7 +777,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -909,7 +891,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,11 +953,11 @@
       <c r="D10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>41</v>
+      <c r="E10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -984,14 +966,14 @@
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>42</v>
+      <c r="D11" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1000,162 +982,162 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>45</v>
+      <c r="D12" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>